<commit_message>
Starting the results analisys
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Classes</t>
   </si>
@@ -36,87 +36,39 @@
     <t>General LOC</t>
   </si>
   <si>
-    <t>General WMC</t>
-  </si>
-  <si>
     <t>General LOCFanIn</t>
   </si>
   <si>
-    <t>General WMCFanIn</t>
-  </si>
-  <si>
     <t>General AtClassScope LOC</t>
   </si>
   <si>
-    <t>General AtClassScope WMC</t>
-  </si>
-  <si>
     <t>General AtClassScope LOCFanIn</t>
   </si>
   <si>
-    <t>General AtClassScope WMCFanIn</t>
-  </si>
-  <si>
     <t>General AtPackageScope LOC</t>
   </si>
   <si>
-    <t>General AtPackageScope WMC</t>
-  </si>
-  <si>
     <t>General AtPackageScope LOCFanIn</t>
   </si>
   <si>
-    <t>General AtPackageScope WMCFanIn</t>
-  </si>
-  <si>
-    <t>General AtNamespaceScope LOC</t>
-  </si>
-  <si>
-    <t>General AtNamespaceScope WMC</t>
-  </si>
-  <si>
-    <t>General AtNamespaceScope LOCFanIn</t>
-  </si>
-  <si>
-    <t>General AtNamespaceScope WMCFanIn</t>
-  </si>
-  <si>
     <t>Invocations LOC</t>
   </si>
   <si>
-    <t>Invocations WMC</t>
-  </si>
-  <si>
     <t>Invocations LOCFanIn</t>
   </si>
   <si>
-    <t>Invocations WMCFanIn</t>
-  </si>
-  <si>
     <t>Invocations AtClassScope LOC</t>
   </si>
   <si>
-    <t>Invocations AtClassScope WMC</t>
-  </si>
-  <si>
     <t>Invocations AtClassScope LOCFanIn</t>
   </si>
   <si>
-    <t>Invocations AtClassScope WMCFanIn</t>
-  </si>
-  <si>
     <t>Invocations AtPackageScope LOC</t>
   </si>
   <si>
-    <t>Invocations AtPackageScope WMC</t>
-  </si>
-  <si>
     <t>Invocations AtPackageScope LOCFanIn</t>
   </si>
   <si>
-    <t>Invocations AtPackageScope WMCFanIn</t>
-  </si>
-  <si>
     <t>Methods</t>
   </si>
   <si>
@@ -157,6 +109,90 @@
   </si>
   <si>
     <t>Packages</t>
+  </si>
+  <si>
+    <t>AD-LOC</t>
+  </si>
+  <si>
+    <t>AD-WMC</t>
+  </si>
+  <si>
+    <t>OI-LOC</t>
+  </si>
+  <si>
+    <t>OI-WMC</t>
+  </si>
+  <si>
+    <t>AD-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>AD-WMC/FanIn</t>
+  </si>
+  <si>
+    <t>AD/ACS-LOC</t>
+  </si>
+  <si>
+    <t>AD/ACS-WMC</t>
+  </si>
+  <si>
+    <t>AD/ACS-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>AD/ACS-WMC/FanIn</t>
+  </si>
+  <si>
+    <t>AD/APS-LOC</t>
+  </si>
+  <si>
+    <t>AD/APS-WMC</t>
+  </si>
+  <si>
+    <t>AD/APS-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>AD/APS-WMC/FanIn</t>
+  </si>
+  <si>
+    <t>AD/ANS-LOC</t>
+  </si>
+  <si>
+    <t>AD/ANS-WMC</t>
+  </si>
+  <si>
+    <t>AD/ANS-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>AD/ANS-WMC/FanIn</t>
+  </si>
+  <si>
+    <t>OI-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>OI-WMC/FanIn</t>
+  </si>
+  <si>
+    <t>OI/ACS-LOC</t>
+  </si>
+  <si>
+    <t>OI/ACS-WMC</t>
+  </si>
+  <si>
+    <t>OI/ACS-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>OI/ACS-WMC/FanIn</t>
+  </si>
+  <si>
+    <t>OI/APS-LOC</t>
+  </si>
+  <si>
+    <t>OI/APS-WMC</t>
+  </si>
+  <si>
+    <t>OI/APS-LOC/FanIn</t>
+  </si>
+  <si>
+    <t>OI/APS-WMC/FanIn</t>
   </si>
 </sst>
 </file>
@@ -305,18 +341,19 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -332,107 +369,93 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$3:$A$30</c:f>
+              <c:f>(Hoja1!$A$3:$A$14,Hoja1!$A$19:$A$30)</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>General LOC</c:v>
+                  <c:v>AD-LOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>General WMC</c:v>
+                  <c:v>AD-WMC</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>General LOCFanIn</c:v>
+                  <c:v>AD-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>General WMCFanIn</c:v>
+                  <c:v>AD-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>General AtClassScope LOC</c:v>
+                  <c:v>AD/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>General AtClassScope WMC</c:v>
+                  <c:v>AD/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>General AtClassScope LOCFanIn</c:v>
+                  <c:v>AD/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>General AtClassScope WMCFanIn</c:v>
+                  <c:v>AD/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>General AtPackageScope LOC</c:v>
+                  <c:v>AD/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>General AtPackageScope WMC</c:v>
+                  <c:v>AD/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>General AtPackageScope LOCFanIn</c:v>
+                  <c:v>AD/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>General AtPackageScope WMCFanIn</c:v>
+                  <c:v>AD/APS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>General AtNamespaceScope LOC</c:v>
+                  <c:v>OI-LOC</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>General AtNamespaceScope WMC</c:v>
+                  <c:v>OI-WMC</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>General AtNamespaceScope LOCFanIn</c:v>
+                  <c:v>OI-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>General AtNamespaceScope WMCFanIn</c:v>
+                  <c:v>OI-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Invocations LOC</c:v>
+                  <c:v>OI/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Invocations WMC</c:v>
+                  <c:v>OI/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Invocations LOCFanIn</c:v>
+                  <c:v>OI/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Invocations WMCFanIn</c:v>
+                  <c:v>OI/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Invocations AtClassScope LOC</c:v>
+                  <c:v>OI/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Invocations AtClassScope WMC</c:v>
+                  <c:v>OI/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Invocations AtClassScope LOCFanIn</c:v>
+                  <c:v>OI/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Invocations AtClassScope WMCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Invocations AtPackageScope LOC</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Invocations AtPackageScope WMC</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Invocations AtPackageScope LOCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Invocations AtPackageScope WMCFanIn</c:v>
+                  <c:v>OI/APS-WMC/FanIn</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$30</c:f>
+              <c:f>(Hoja1!$B$3:$B$14,Hoja1!$B$19:$B$30)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.84379999999999999</c:v>
                 </c:pt>
@@ -470,57 +493,44 @@
                   <c:v>0.21820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.3E-3</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>4.0000000000000003E-5</c:v>
+                  <c:v>0.84189999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.62639999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.2299999999999997E-2</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.3300000000000003E-2</c:v>
+                  <c:v>5.9999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.84189999999999998</c:v>
+                  <c:v>0.2283</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.62639999999999996</c:v>
+                  <c:v>0.35010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1E-3</c:v>
+                  <c:v>0.26050000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9999999999999995E-4</c:v>
+                  <c:v>0.2389</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2283</c:v>
+                  <c:v>0.20810000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.35010000000000002</c:v>
+                  <c:v>0.36459999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.26050000000000001</c:v>
+                  <c:v>0.26960000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.2389</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.20810000000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.36459999999999998</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.26960000000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>0.2384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -536,107 +546,93 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$3:$A$30</c:f>
+              <c:f>(Hoja1!$A$3:$A$14,Hoja1!$A$19:$A$30)</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>General LOC</c:v>
+                  <c:v>AD-LOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>General WMC</c:v>
+                  <c:v>AD-WMC</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>General LOCFanIn</c:v>
+                  <c:v>AD-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>General WMCFanIn</c:v>
+                  <c:v>AD-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>General AtClassScope LOC</c:v>
+                  <c:v>AD/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>General AtClassScope WMC</c:v>
+                  <c:v>AD/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>General AtClassScope LOCFanIn</c:v>
+                  <c:v>AD/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>General AtClassScope WMCFanIn</c:v>
+                  <c:v>AD/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>General AtPackageScope LOC</c:v>
+                  <c:v>AD/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>General AtPackageScope WMC</c:v>
+                  <c:v>AD/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>General AtPackageScope LOCFanIn</c:v>
+                  <c:v>AD/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>General AtPackageScope WMCFanIn</c:v>
+                  <c:v>AD/APS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>General AtNamespaceScope LOC</c:v>
+                  <c:v>OI-LOC</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>General AtNamespaceScope WMC</c:v>
+                  <c:v>OI-WMC</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>General AtNamespaceScope LOCFanIn</c:v>
+                  <c:v>OI-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>General AtNamespaceScope WMCFanIn</c:v>
+                  <c:v>OI-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Invocations LOC</c:v>
+                  <c:v>OI/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Invocations WMC</c:v>
+                  <c:v>OI/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Invocations LOCFanIn</c:v>
+                  <c:v>OI/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Invocations WMCFanIn</c:v>
+                  <c:v>OI/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Invocations AtClassScope LOC</c:v>
+                  <c:v>OI/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Invocations AtClassScope WMC</c:v>
+                  <c:v>OI/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Invocations AtClassScope LOCFanIn</c:v>
+                  <c:v>OI/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Invocations AtClassScope WMCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Invocations AtPackageScope LOC</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Invocations AtPackageScope WMC</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Invocations AtPackageScope LOCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Invocations AtPackageScope WMCFanIn</c:v>
+                  <c:v>OI/APS-WMC/FanIn</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$3:$C$30</c:f>
+              <c:f>(Hoja1!$C$3:$C$14,Hoja1!$C$19:$C$30)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.94079999999999997</c:v>
                 </c:pt>
@@ -674,57 +670,44 @@
                   <c:v>0.23549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.3000000000000001E-3</c:v>
+                  <c:v>0.95269999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.3799999999999999E-2</c:v>
+                  <c:v>0.50419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.2000000000000007E-3</c:v>
+                  <c:v>0.15210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.21E-2</c:v>
+                  <c:v>0.14849999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.95269999999999999</c:v>
+                  <c:v>4.2700000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.50419999999999998</c:v>
+                  <c:v>0.1149</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.15210000000000001</c:v>
+                  <c:v>0.25230000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.14849999999999999</c:v>
+                  <c:v>0.2281</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.2700000000000002E-2</c:v>
+                  <c:v>7.4499999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.1149</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.25230000000000002</c:v>
+                  <c:v>0.1842</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.2281</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.4499999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.122</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.1842</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>0.18160000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -740,107 +723,93 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$3:$A$30</c:f>
+              <c:f>(Hoja1!$A$3:$A$14,Hoja1!$A$19:$A$30)</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>General LOC</c:v>
+                  <c:v>AD-LOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>General WMC</c:v>
+                  <c:v>AD-WMC</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>General LOCFanIn</c:v>
+                  <c:v>AD-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>General WMCFanIn</c:v>
+                  <c:v>AD-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>General AtClassScope LOC</c:v>
+                  <c:v>AD/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>General AtClassScope WMC</c:v>
+                  <c:v>AD/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>General AtClassScope LOCFanIn</c:v>
+                  <c:v>AD/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>General AtClassScope WMCFanIn</c:v>
+                  <c:v>AD/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>General AtPackageScope LOC</c:v>
+                  <c:v>AD/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>General AtPackageScope WMC</c:v>
+                  <c:v>AD/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>General AtPackageScope LOCFanIn</c:v>
+                  <c:v>AD/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>General AtPackageScope WMCFanIn</c:v>
+                  <c:v>AD/APS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>General AtNamespaceScope LOC</c:v>
+                  <c:v>OI-LOC</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>General AtNamespaceScope WMC</c:v>
+                  <c:v>OI-WMC</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>General AtNamespaceScope LOCFanIn</c:v>
+                  <c:v>OI-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>General AtNamespaceScope WMCFanIn</c:v>
+                  <c:v>OI-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Invocations LOC</c:v>
+                  <c:v>OI/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Invocations WMC</c:v>
+                  <c:v>OI/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Invocations LOCFanIn</c:v>
+                  <c:v>OI/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Invocations WMCFanIn</c:v>
+                  <c:v>OI/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Invocations AtClassScope LOC</c:v>
+                  <c:v>OI/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Invocations AtClassScope WMC</c:v>
+                  <c:v>OI/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Invocations AtClassScope LOCFanIn</c:v>
+                  <c:v>OI/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Invocations AtClassScope WMCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Invocations AtPackageScope LOC</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Invocations AtPackageScope WMC</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Invocations AtPackageScope LOCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Invocations AtPackageScope WMCFanIn</c:v>
+                  <c:v>OI/APS-WMC/FanIn</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$30</c:f>
+              <c:f>(Hoja1!$D$3:$D$14,Hoja1!$D$19:$D$30)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.86580000000000001</c:v>
                 </c:pt>
@@ -878,57 +847,44 @@
                   <c:v>7.0499999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.9600000000000004E-2</c:v>
+                  <c:v>0.88859999999999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.75E-2</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>3.0000000000000001E-6</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>1.0000000000000001E-5</c:v>
+                  <c:v>0.81499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1794</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15709999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.88859999999999995</c:v>
+                  <c:v>0.70640000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.81499999999999995</c:v>
+                  <c:v>0.58169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.1794</c:v>
+                  <c:v>0.1331</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.15709999999999999</c:v>
+                  <c:v>0.1081</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.70640000000000003</c:v>
+                  <c:v>0.44059999999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.58169999999999999</c:v>
+                  <c:v>0.29909999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.1331</c:v>
+                  <c:v>8.8700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.1081</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.44059999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.29909999999999998</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.8700000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -944,107 +900,93 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$3:$A$30</c:f>
+              <c:f>(Hoja1!$A$3:$A$14,Hoja1!$A$19:$A$30)</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>General LOC</c:v>
+                  <c:v>AD-LOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>General WMC</c:v>
+                  <c:v>AD-WMC</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>General LOCFanIn</c:v>
+                  <c:v>AD-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>General WMCFanIn</c:v>
+                  <c:v>AD-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>General AtClassScope LOC</c:v>
+                  <c:v>AD/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>General AtClassScope WMC</c:v>
+                  <c:v>AD/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>General AtClassScope LOCFanIn</c:v>
+                  <c:v>AD/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>General AtClassScope WMCFanIn</c:v>
+                  <c:v>AD/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>General AtPackageScope LOC</c:v>
+                  <c:v>AD/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>General AtPackageScope WMC</c:v>
+                  <c:v>AD/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>General AtPackageScope LOCFanIn</c:v>
+                  <c:v>AD/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>General AtPackageScope WMCFanIn</c:v>
+                  <c:v>AD/APS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>General AtNamespaceScope LOC</c:v>
+                  <c:v>OI-LOC</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>General AtNamespaceScope WMC</c:v>
+                  <c:v>OI-WMC</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>General AtNamespaceScope LOCFanIn</c:v>
+                  <c:v>OI-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>General AtNamespaceScope WMCFanIn</c:v>
+                  <c:v>OI-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Invocations LOC</c:v>
+                  <c:v>OI/ACS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Invocations WMC</c:v>
+                  <c:v>OI/ACS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Invocations LOCFanIn</c:v>
+                  <c:v>OI/ACS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Invocations WMCFanIn</c:v>
+                  <c:v>OI/ACS-WMC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Invocations AtClassScope LOC</c:v>
+                  <c:v>OI/APS-LOC</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Invocations AtClassScope WMC</c:v>
+                  <c:v>OI/APS-WMC</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Invocations AtClassScope LOCFanIn</c:v>
+                  <c:v>OI/APS-LOC/FanIn</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Invocations AtClassScope WMCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Invocations AtPackageScope LOC</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Invocations AtPackageScope WMC</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Invocations AtPackageScope LOCFanIn</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Invocations AtPackageScope WMCFanIn</c:v>
+                  <c:v>OI/APS-WMC/FanIn</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$30</c:f>
+              <c:f>(Hoja1!$E$3:$E$14,Hoja1!$E$19:$E$30)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.79879999999999995</c:v>
                 </c:pt>
@@ -1082,57 +1024,44 @@
                   <c:v>5.7799999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9600000000000001E-2</c:v>
+                  <c:v>0.66920000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.49E-2</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1.0000000000000001E-5</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>3.0000000000000001E-5</c:v>
+                  <c:v>0.53369999999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29980000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.30780000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.66920000000000002</c:v>
+                  <c:v>0.54930000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.53369999999999995</c:v>
+                  <c:v>0.4748</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29980000000000001</c:v>
+                  <c:v>0.13489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.30780000000000002</c:v>
+                  <c:v>0.1477</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.54930000000000001</c:v>
+                  <c:v>0.28210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.4748</c:v>
+                  <c:v>0.19359999999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.13489999999999999</c:v>
+                  <c:v>5.8900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.1477</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.28210000000000002</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.19359999999999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.8900000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
                   <c:v>6.3600000000000004E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1142,13 +1071,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="62793216"/>
-        <c:axId val="195548224"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="97225728"/>
+        <c:axId val="58599104"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="62793216"/>
+        <c:axId val="97225728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,7 +1085,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195548224"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58599104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1165,9 +1103,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195548224"/>
+        <c:axId val="58599104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1176,7 +1115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62793216"/>
+        <c:crossAx val="97225728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,8 +1131,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1948,11 +1887,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139486720"/>
-        <c:axId val="191990592"/>
+        <c:axId val="41570816"/>
+        <c:axId val="58603712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139486720"/>
+        <c:axId val="41570816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1961,7 +1900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191990592"/>
+        <c:crossAx val="58603712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1969,7 +1908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191990592"/>
+        <c:axId val="58603712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +1919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139486720"/>
+        <c:crossAx val="41570816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2752,11 +2691,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="203616256"/>
-        <c:axId val="221505216"/>
+        <c:axId val="41684992"/>
+        <c:axId val="41487168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203616256"/>
+        <c:axId val="41684992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2765,7 +2704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221505216"/>
+        <c:crossAx val="41487168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2773,7 +2712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221505216"/>
+        <c:axId val="41487168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2784,7 +2723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203616256"/>
+        <c:crossAx val="41684992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2811,15 +2750,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>347662</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2846,15 +2785,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>209549</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>400049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2881,15 +2820,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3200,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3230,9 +3169,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3">
         <v>0.84379999999999999</v>
@@ -3249,7 +3188,7 @@
     </row>
     <row r="4" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>0.64159999999999995</v>
@@ -3266,7 +3205,7 @@
     </row>
     <row r="5" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>3.2000000000000002E-3</v>
@@ -3283,7 +3222,7 @@
     </row>
     <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>2.2000000000000001E-3</v>
@@ -3298,9 +3237,9 @@
         <v>0.3216</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3">
         <v>0.3695</v>
@@ -3315,9 +3254,9 @@
         <v>0.58279999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3">
         <v>0.53510000000000002</v>
@@ -3332,9 +3271,9 @@
         <v>0.51090000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3">
         <v>0.30470000000000003</v>
@@ -3349,9 +3288,9 @@
         <v>0.1469</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
         <v>0.26179999999999998</v>
@@ -3366,9 +3305,9 @@
         <v>0.1615</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3">
         <v>0.39219999999999999</v>
@@ -3383,9 +3322,9 @@
         <v>0.2707</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3">
         <v>0.53400000000000003</v>
@@ -3400,9 +3339,9 @@
         <v>0.17979999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3">
         <v>0.25979999999999998</v>
@@ -3417,9 +3356,9 @@
         <v>5.4399999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3">
         <v>0.21820000000000001</v>
@@ -3434,9 +3373,9 @@
         <v>5.7799999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3">
         <v>5.3E-3</v>
@@ -3451,9 +3390,9 @@
         <v>2.9600000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B16" s="4">
         <v>4.0000000000000003E-5</v>
@@ -3468,9 +3407,9 @@
         <v>1.49E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3">
         <v>4.2299999999999997E-2</v>
@@ -3485,9 +3424,9 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3">
         <v>3.3300000000000003E-2</v>
@@ -3504,7 +3443,7 @@
     </row>
     <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3">
         <v>0.84189999999999998</v>
@@ -3521,7 +3460,7 @@
     </row>
     <row r="20" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3">
         <v>0.62639999999999996</v>
@@ -3538,7 +3477,7 @@
     </row>
     <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3">
         <v>1E-3</v>
@@ -3555,7 +3494,7 @@
     </row>
     <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3">
         <v>5.9999999999999995E-4</v>
@@ -3570,9 +3509,9 @@
         <v>0.30780000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3">
         <v>0.2283</v>
@@ -3587,9 +3526,9 @@
         <v>0.54930000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3">
         <v>0.35010000000000002</v>
@@ -3604,9 +3543,9 @@
         <v>0.4748</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3">
         <v>0.26050000000000001</v>
@@ -3621,9 +3560,9 @@
         <v>0.13489999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3">
         <v>0.2389</v>
@@ -3638,9 +3577,9 @@
         <v>0.1477</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3">
         <v>0.20810000000000001</v>
@@ -3655,9 +3594,9 @@
         <v>0.28210000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3">
         <v>0.36459999999999998</v>
@@ -3672,9 +3611,9 @@
         <v>0.19359999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3">
         <v>0.26960000000000001</v>
@@ -3689,9 +3628,9 @@
         <v>5.8900000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3">
         <v>0.2384</v>
@@ -3728,7 +3667,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -3769,7 +3708,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>0.1363</v>
@@ -3786,7 +3725,7 @@
     </row>
     <row r="5" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>2.5899999999999999E-2</v>
@@ -3803,7 +3742,7 @@
     </row>
     <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3">
         <v>8.5000000000000006E-3</v>
@@ -3820,7 +3759,7 @@
     </row>
     <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>2.5000000000000001E-3</v>
@@ -3837,7 +3776,7 @@
     </row>
     <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
         <v>2.6599999999999999E-2</v>
@@ -3854,7 +3793,7 @@
     </row>
     <row r="9" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>1.9999999999999999E-6</v>
@@ -3871,7 +3810,7 @@
     </row>
     <row r="10" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3">
         <v>2.9999999999999997E-4</v>
@@ -3888,7 +3827,7 @@
     </row>
     <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>8.0000000000000002E-3</v>
@@ -3905,7 +3844,7 @@
     </row>
     <row r="12" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3">
         <v>1.2200000000000001E-2</v>
@@ -3922,7 +3861,7 @@
     </row>
     <row r="13" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>5.0000000000000001E-4</v>
@@ -3939,7 +3878,7 @@
     </row>
     <row r="14" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4">
         <v>3.9999999999999998E-6</v>
@@ -3956,7 +3895,7 @@
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3">
         <v>2.0000000000000001E-4</v>
@@ -3973,7 +3912,7 @@
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3">
         <v>3.78E-2</v>
@@ -3990,7 +3929,7 @@
     </row>
     <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
         <v>1.1299999999999999E-2</v>
@@ -4007,7 +3946,7 @@
     </row>
     <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3">
         <v>3.0999999999999999E-3</v>
@@ -4024,7 +3963,7 @@
     </row>
     <row r="19" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3">
         <v>3.0000000000000001E-3</v>
@@ -4041,7 +3980,7 @@
     </row>
     <row r="20" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3">
         <v>3.5099999999999999E-2</v>
@@ -4058,7 +3997,7 @@
     </row>
     <row r="21" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4">
         <v>3.0000000000000001E-5</v>
@@ -4075,7 +4014,7 @@
     </row>
     <row r="22" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3">
         <v>2.0000000000000001E-4</v>
@@ -4092,7 +4031,7 @@
     </row>
     <row r="23" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B23" s="3">
         <v>9.9000000000000008E-3</v>
@@ -4109,7 +4048,7 @@
     </row>
     <row r="24" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>1.52E-2</v>
@@ -4126,7 +4065,7 @@
     </row>
     <row r="25" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
         <v>1.6999999999999999E-3</v>
@@ -4143,7 +4082,7 @@
     </row>
     <row r="26" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B26" s="3">
         <v>2.0000000000000001E-4</v>
@@ -4171,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,7 +4121,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -4223,7 +4162,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>0.52</v>
@@ -4240,7 +4179,7 @@
     </row>
     <row r="5" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>0.77459999999999996</v>
@@ -4257,7 +4196,7 @@
     </row>
     <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3">
         <v>0.1119</v>
@@ -4274,7 +4213,7 @@
     </row>
     <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>0.54300000000000004</v>
@@ -4291,7 +4230,7 @@
     </row>
     <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
         <v>0.62809999999999999</v>
@@ -4308,7 +4247,7 @@
     </row>
     <row r="9" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>0.68879999999999997</v>
@@ -4325,7 +4264,7 @@
     </row>
     <row r="10" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3">
         <v>0.43290000000000001</v>
@@ -4342,7 +4281,7 @@
     </row>
     <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>0.35649999999999998</v>
@@ -4359,7 +4298,7 @@
     </row>
     <row r="12" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3">
         <v>0.18840000000000001</v>
@@ -4376,7 +4315,7 @@
     </row>
     <row r="13" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>0.249</v>
@@ -4393,7 +4332,7 @@
     </row>
     <row r="14" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3">
         <v>3.7999999999999999E-2</v>
@@ -4410,7 +4349,7 @@
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3">
         <v>0.95899999999999996</v>
@@ -4427,7 +4366,7 @@
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3">
         <v>0.49859999999999999</v>
@@ -4444,7 +4383,7 @@
     </row>
     <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
         <v>0.76659999999999995</v>
@@ -4461,7 +4400,7 @@
     </row>
     <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3">
         <v>0.1023</v>
@@ -4478,7 +4417,7 @@
     </row>
     <row r="19" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3">
         <v>0.3629</v>
@@ -4495,7 +4434,7 @@
     </row>
     <row r="20" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3">
         <v>0.64319999999999999</v>
@@ -4512,7 +4451,7 @@
     </row>
     <row r="21" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B21" s="3">
         <v>0.60009999999999997</v>
@@ -4529,7 +4468,7 @@
     </row>
     <row r="22" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3">
         <v>0.56969999999999998</v>
@@ -4546,7 +4485,7 @@
     </row>
     <row r="23" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B23" s="3">
         <v>0.35099999999999998</v>
@@ -4563,7 +4502,7 @@
     </row>
     <row r="24" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>0.45100000000000001</v>
@@ -4580,7 +4519,7 @@
     </row>
     <row r="25" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
         <v>0.36520000000000002</v>
@@ -4597,7 +4536,7 @@
     </row>
     <row r="26" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B26" s="3">
         <v>0.2417</v>

</xml_diff>